<commit_message>
col perc for table 2
</commit_message>
<xml_diff>
--- a/Index.xlsx
+++ b/Index.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmenrodriguez/Desktop/Research Projects/BayesBinMix/ecbayesbinmix/Model Outputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carmenrodriguez/Desktop/Research Projects/BayesBinMix/ecbayesbinmix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15D596F-BB8F-3C40-89C1-106744069312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E09D206-8E49-AF4D-84B1-9439067009AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16780" yWindow="500" windowWidth="21620" windowHeight="21100" activeTab="1" xr2:uid="{1332027C-E688-B74E-83F2-51C559BB0914}"/>
+    <workbookView xWindow="1820" yWindow="500" windowWidth="26340" windowHeight="17500" activeTab="1" xr2:uid="{1332027C-E688-B74E-83F2-51C559BB0914}"/>
   </bookViews>
   <sheets>
     <sheet name="Model_output" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -153,7 +153,13 @@
     <t>ISBA 2024 poster presentation</t>
   </si>
   <si>
-    <t>Code for manuscript- only inlcudes last survey wave</t>
+    <t>Code for manuscript- only inlcudes last survey wave model results</t>
+  </si>
+  <si>
+    <t>/Users/carmenrodriguez/Desktop/Research Projects/BayesBinMix/ecbayesbinmix/ECbayesbinmix_manuscript.R</t>
+  </si>
+  <si>
+    <t>Code for manuscript- EC data and Bayesbinmix resutls</t>
   </si>
 </sst>
 </file>
@@ -755,7 +761,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -837,9 +843,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
+    <row r="10" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>

</xml_diff>